<commit_message>
breakdown + fibonaci BE
</commit_message>
<xml_diff>
--- a/our-notes/Breakdown Notifikasi.xlsx
+++ b/our-notes/Breakdown Notifikasi.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Git\belajarJadiPedagang\our-notes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1170" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -21,20 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="30">
   <si>
     <t>send email</t>
   </si>
   <si>
-    <t>Revisi Database</t>
-  </si>
-  <si>
-    <t>buat/edit table</t>
-  </si>
-  <si>
-    <t>sekalian buat dokumentasi, sequence nya</t>
-  </si>
-  <si>
     <t>controller, entity, service, mapper</t>
   </si>
   <si>
@@ -53,15 +39,9 @@
     <t>Compose email and email history/mailing list</t>
   </si>
   <si>
-    <t>api for sender_config (insert, delete, edit, get all(list), get by id)</t>
-  </si>
-  <si>
     <t>master parameter - email template category</t>
   </si>
   <si>
-    <t>api for email template category (insert, delete, edit, get all(list), get by id)</t>
-  </si>
-  <si>
     <t>email template</t>
   </si>
   <si>
@@ -71,15 +51,9 @@
     <t>controller, service</t>
   </si>
   <si>
-    <t>api for email template (insert, delete, edit, get all(list), get by id, pagination) - ngereference dari email template recipient</t>
-  </si>
-  <si>
     <t>dibagian insert : return id email template untuk preview template</t>
   </si>
   <si>
-    <t>api for email history (insert, get all(list), get by id, pagination)</t>
-  </si>
-  <si>
     <t>NOTIFICATION BREAKDOWN - BE</t>
   </si>
   <si>
@@ -96,6 +70,42 @@
   </si>
   <si>
     <t>FIBONACCI</t>
+  </si>
+  <si>
+    <t>api for email history (insert, get all(list), get by id)</t>
+  </si>
+  <si>
+    <t>pagination</t>
+  </si>
+  <si>
+    <t>table, controller, entity, service, mapper</t>
+  </si>
+  <si>
+    <t>api for email template (insert,get all(list), get by id) - ngereference dari email template recipient</t>
+  </si>
+  <si>
+    <t>api for email template (delete, edit) - ngereference dari email template recipient</t>
+  </si>
+  <si>
+    <t>save sent email to email history/mailing list</t>
+  </si>
+  <si>
+    <t>controller, service, mapper</t>
+  </si>
+  <si>
+    <t>Send email with template</t>
+  </si>
+  <si>
+    <t>api for sender_config (delete, edit)</t>
+  </si>
+  <si>
+    <t>api for sender_config (insert,get all(list), get by id)</t>
+  </si>
+  <si>
+    <t>api for email template category (delete, edit)</t>
+  </si>
+  <si>
+    <t>api for email template category (insert, get all(list), get by id)</t>
   </si>
 </sst>
 </file>
@@ -150,15 +160,6 @@
   <borders count="9">
     <border>
       <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
       <right/>
       <top/>
       <bottom/>
@@ -241,35 +242,74 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -277,20 +317,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -352,7 +380,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -387,7 +415,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -596,268 +624,356 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:F26"/>
+  <dimension ref="B1:F32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="9.140625" style="1"/>
+    <col min="1" max="1" width="9.140625" style="1"/>
+    <col min="2" max="2" width="9.140625" style="19"/>
     <col min="3" max="3" width="37.28515625" style="1" customWidth="1"/>
     <col min="4" max="4" width="54.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="37" style="1" customWidth="1"/>
+    <col min="5" max="5" width="40.85546875" style="1" customWidth="1"/>
     <col min="6" max="6" width="12.28515625" style="1" customWidth="1"/>
     <col min="7" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="F3" s="13" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="7">
+        <v>1</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F4" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="7"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" s="2" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+      <c r="B6" s="7">
+        <v>2</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F6" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4" t="s">
+        <v>0</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="F7" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="7"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F8" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="7"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="7"/>
-      <c r="D1" s="7"/>
-      <c r="E1" s="7"/>
-      <c r="F1" s="7"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" s="11" t="s">
+      <c r="E9" s="4"/>
+      <c r="F9" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="7"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B11" s="6">
+        <v>3</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="7"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="E12" s="4"/>
+      <c r="F12" s="4">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B13" s="7">
+        <v>4</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>8</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F13" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B14" s="7"/>
+      <c r="C14" s="15"/>
+      <c r="D14" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="F14" s="15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="7"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="B16" s="7"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="4"/>
+      <c r="E16" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="4"/>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="7">
+        <v>5</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="17"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="C3" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D3" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="11" t="s">
+      <c r="E18" s="5" t="s">
         <v>24</v>
       </c>
-    </row>
-    <row r="4" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B4" s="8">
+      <c r="F18" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="18"/>
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="1">
+        <f>SUM(F4:F18)</f>
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B21" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="14"/>
+      <c r="E21" s="14"/>
+      <c r="F21" s="14"/>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="F23" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="6">
         <v>1</v>
       </c>
-      <c r="C4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="D4" s="4" t="s">
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="7">
         <v>2</v>
       </c>
-      <c r="E4" s="4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" s="13"/>
-    </row>
-    <row r="5" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B5" s="9">
-        <v>2</v>
-      </c>
-      <c r="C5" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="E5" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F5" s="14"/>
-    </row>
-    <row r="6" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B6" s="9">
-        <v>3</v>
-      </c>
-      <c r="C6" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="D6" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="E6" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="F6" s="14"/>
-    </row>
-    <row r="7" spans="2:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B7" s="9"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="E7" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="F7" s="14"/>
-    </row>
-    <row r="8" spans="2:6" s="3" customFormat="1" ht="30" x14ac:dyDescent="0.25">
-      <c r="B8" s="10"/>
-      <c r="C8" s="6"/>
-      <c r="D8" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B9" s="9">
-        <v>4</v>
-      </c>
-      <c r="C9" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="D9" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="E9" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="13"/>
-    </row>
-    <row r="10" spans="2:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B10" s="9">
-        <v>5</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="D10" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="E10" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="14"/>
-    </row>
-    <row r="11" spans="2:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="5"/>
-      <c r="E11" s="5" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="14"/>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" s="6"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="5" t="s">
-        <v>14</v>
-      </c>
-      <c r="E12" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="12"/>
-      <c r="D13" s="12"/>
-      <c r="E13" s="12"/>
-    </row>
-    <row r="15" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B15" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="C15" s="7"/>
-      <c r="D15" s="7"/>
-      <c r="E15" s="7"/>
-      <c r="F15" s="7"/>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B17" s="11" t="s">
-        <v>23</v>
-      </c>
-      <c r="C17" s="11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17" s="11" t="s">
-        <v>21</v>
-      </c>
-      <c r="E17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="F17" s="11" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B18" s="8">
-        <v>1</v>
-      </c>
-      <c r="C18" s="4"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="13"/>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B19" s="9">
-        <v>2</v>
-      </c>
-      <c r="C19" s="5"/>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="14"/>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B20" s="9">
-        <v>3</v>
-      </c>
-      <c r="C20" s="5"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="14"/>
-    </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B21" s="9"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="14"/>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="9"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="14"/>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="9"/>
-      <c r="C23" s="5"/>
-      <c r="D23" s="5"/>
-      <c r="E23" s="5"/>
-      <c r="F23" s="5"/>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B24" s="9"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="14"/>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B25" s="5"/>
-      <c r="C25" s="5"/>
-      <c r="E25" s="5"/>
-      <c r="F25" s="14"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="4"/>
+      <c r="E25" s="4"/>
+      <c r="F25" s="11"/>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B26" s="6"/>
-      <c r="C26" s="6"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="15"/>
+      <c r="B26" s="7">
+        <v>3</v>
+      </c>
+      <c r="C26" s="4"/>
+      <c r="D26" s="4"/>
+      <c r="E26" s="4"/>
+      <c r="F26" s="11"/>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="7"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="4"/>
+      <c r="E27" s="4"/>
+      <c r="F27" s="11"/>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="7"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="4"/>
+      <c r="E28" s="4"/>
+      <c r="F28" s="11"/>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="7"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="4"/>
+      <c r="E29" s="4"/>
+      <c r="F29" s="4"/>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="7"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="4"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="11"/>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="7"/>
+      <c r="C31" s="4"/>
+      <c r="E31" s="4"/>
+      <c r="F31" s="11"/>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="17"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="B1:F1"/>
-    <mergeCell ref="B15:F15"/>
+    <mergeCell ref="B21:F21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>

<commit_message>
Revisi dikit di Add email Category
</commit_message>
<xml_diff>
--- a/our-notes/Breakdown Notifikasi.xlsx
+++ b/our-notes/Breakdown Notifikasi.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ulfair\Documents\belajarJadiPedagang\our-notes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="1170" yWindow="60" windowWidth="20115" windowHeight="8010"/>
   </bookViews>
@@ -11,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -165,9 +170,6 @@
     <t>Action Edit : menampilkan form edit untuk mengubah template email category</t>
   </si>
   <si>
-    <t xml:space="preserve">Add email template category (field berupa : Category,  Description, Status, button submit and cancel) </t>
-  </si>
-  <si>
     <t>History List</t>
   </si>
   <si>
@@ -175,6 +177,9 @@
   </si>
   <si>
     <t>controller, pagination, event pada button dan filter(sort)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Add email template category (field berupa : Category,  Description, button submit and cancel) </t>
   </si>
 </sst>
 </file>
@@ -395,9 +400,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -423,6 +425,9 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -485,7 +490,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -520,7 +525,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -731,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
+      <selection activeCell="D34" sqref="D34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -747,13 +752,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:6" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="25" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="16"/>
-      <c r="D1" s="16"/>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="C1" s="25"/>
+      <c r="D1" s="25"/>
+      <c r="E1" s="25"/>
+      <c r="F1" s="25"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B3" s="10" t="s">
@@ -982,13 +987,13 @@
       </c>
     </row>
     <row r="21" spans="2:6" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="25" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="16"/>
-      <c r="D21" s="16"/>
-      <c r="E21" s="16"/>
-      <c r="F21" s="16"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
+      <c r="E21" s="25"/>
+      <c r="F21" s="25"/>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="1"/>
@@ -1023,7 +1028,7 @@
       <c r="E24" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="17">
+      <c r="F24" s="16">
         <v>3</v>
       </c>
     </row>
@@ -1040,33 +1045,33 @@
       <c r="E25" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="F25" s="18">
+      <c r="F25" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="26" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
-      <c r="D26" s="19" t="s">
+      <c r="D26" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F26" s="18">
+      <c r="F26" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="27" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B27" s="7"/>
       <c r="C27" s="4"/>
-      <c r="D27" s="20" t="s">
+      <c r="D27" s="19" t="s">
         <v>39</v>
       </c>
       <c r="E27" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F27" s="18">
+      <c r="F27" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1077,52 +1082,52 @@
       <c r="C28" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="21" t="s">
+      <c r="D28" s="20" t="s">
         <v>41</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="F28" s="17">
+      <c r="F28" s="16">
         <v>2</v>
       </c>
     </row>
     <row r="29" spans="2:6" ht="48" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="7"/>
       <c r="C29" s="4"/>
-      <c r="D29" s="20" t="s">
+      <c r="D29" s="19" t="s">
         <v>42</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="F29" s="18">
+      <c r="F29" s="17">
         <v>3</v>
       </c>
     </row>
     <row r="30" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B30" s="7"/>
       <c r="C30" s="4"/>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="21" t="s">
         <v>43</v>
       </c>
       <c r="E30" s="4" t="s">
         <v>44</v>
       </c>
-      <c r="F30" s="18">
+      <c r="F30" s="17">
         <v>1</v>
       </c>
     </row>
     <row r="31" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B31" s="7"/>
       <c r="C31" s="4"/>
-      <c r="D31" s="19" t="s">
+      <c r="D31" s="18" t="s">
         <v>37</v>
       </c>
       <c r="E31" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F31" s="18">
+      <c r="F31" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1139,33 +1144,33 @@
       <c r="E32" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="F32" s="23">
+      <c r="F32" s="22">
         <v>2</v>
       </c>
     </row>
     <row r="33" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B33" s="7"/>
       <c r="C33" s="4"/>
-      <c r="D33" s="19" t="s">
+      <c r="D33" s="18" t="s">
         <v>48</v>
       </c>
       <c r="E33" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F33" s="18">
+      <c r="F33" s="17">
         <v>2</v>
       </c>
     </row>
     <row r="34" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B34" s="7"/>
       <c r="C34" s="4"/>
-      <c r="D34" s="24" t="s">
-        <v>49</v>
+      <c r="D34" s="23" t="s">
+        <v>52</v>
       </c>
       <c r="E34" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="F34" s="18">
+      <c r="F34" s="17">
         <v>2</v>
       </c>
     </row>
@@ -1174,15 +1179,15 @@
         <v>5</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="E35" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F35" s="25">
+      <c r="F35" s="24">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
edit breakdown list rmail sender
</commit_message>
<xml_diff>
--- a/our-notes/Breakdown Notifikasi.xlsx
+++ b/our-notes/Breakdown Notifikasi.xlsx
@@ -128,9 +128,6 @@
     <t>Email Sender</t>
   </si>
   <si>
-    <t>tampilan list email sender dengan struktur tabel berupa : No, Category,  Description, Status, Action (Edit, Delete), add email sender, pagination, filter(sort)</t>
-  </si>
-  <si>
     <t>controller, model, event pada button, routing, pagination, filtering(sort)</t>
   </si>
   <si>
@@ -180,6 +177,9 @@
   </si>
   <si>
     <t xml:space="preserve">Add email template category (field berupa : Category,  Description, button submit and cancel) </t>
+  </si>
+  <si>
+    <t>tampilan list email sender dengan struktur tabel berupa : No, Email, Password, Host, Port, Protocol/Security, Action (edit dan delete)</t>
   </si>
 </sst>
 </file>
@@ -736,8 +736,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B31" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView tabSelected="1" topLeftCell="B19" workbookViewId="0">
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1040,10 +1040,10 @@
         <v>34</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>52</v>
+      </c>
+      <c r="E25" s="4" t="s">
         <v>35</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>36</v>
       </c>
       <c r="F25" s="17">
         <v>2</v>
@@ -1053,10 +1053,10 @@
       <c r="B26" s="7"/>
       <c r="C26" s="4"/>
       <c r="D26" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E26" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="F26" s="17">
         <v>2</v>
@@ -1066,10 +1066,10 @@
       <c r="B27" s="7"/>
       <c r="C27" s="4"/>
       <c r="D27" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E27" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F27" s="17">
         <v>2</v>
@@ -1080,13 +1080,13 @@
         <v>3</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="D28" s="20" t="s">
         <v>40</v>
       </c>
-      <c r="D28" s="20" t="s">
-        <v>41</v>
-      </c>
       <c r="E28" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F28" s="16">
         <v>2</v>
@@ -1096,7 +1096,7 @@
       <c r="B29" s="7"/>
       <c r="C29" s="4"/>
       <c r="D29" s="19" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="E29" s="4" t="s">
         <v>33</v>
@@ -1109,10 +1109,10 @@
       <c r="B30" s="7"/>
       <c r="C30" s="4"/>
       <c r="D30" s="21" t="s">
+        <v>42</v>
+      </c>
+      <c r="E30" s="4" t="s">
         <v>43</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>44</v>
       </c>
       <c r="F30" s="17">
         <v>1</v>
@@ -1122,10 +1122,10 @@
       <c r="B31" s="7"/>
       <c r="C31" s="4"/>
       <c r="D31" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="E31" s="4" t="s">
         <v>37</v>
-      </c>
-      <c r="E31" s="4" t="s">
-        <v>38</v>
       </c>
       <c r="F31" s="17">
         <v>2</v>
@@ -1136,13 +1136,13 @@
         <v>4</v>
       </c>
       <c r="C32" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D32" s="4" t="s">
+      <c r="E32" s="4" t="s">
         <v>46</v>
-      </c>
-      <c r="E32" s="4" t="s">
-        <v>47</v>
       </c>
       <c r="F32" s="22">
         <v>2</v>
@@ -1152,10 +1152,10 @@
       <c r="B33" s="7"/>
       <c r="C33" s="4"/>
       <c r="D33" s="18" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="E33" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F33" s="17">
         <v>2</v>
@@ -1165,10 +1165,10 @@
       <c r="B34" s="7"/>
       <c r="C34" s="4"/>
       <c r="D34" s="23" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="E34" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F34" s="17">
         <v>2</v>
@@ -1179,13 +1179,13 @@
         <v>5</v>
       </c>
       <c r="C35" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D35" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="E35" s="5" t="s">
         <v>50</v>
-      </c>
-      <c r="E35" s="5" t="s">
-        <v>51</v>
       </c>
       <c r="F35" s="24">
         <v>2</v>

</xml_diff>